<commit_message>
Manutenção nos cenários existentes
</commit_message>
<xml_diff>
--- a/src/test/java/system/resources/data/cadastro_pessoa_fisica.xlsx
+++ b/src/test/java/system/resources/data/cadastro_pessoa_fisica.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>NOME_DESTINATARIO</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>alexsantos_13032022150114@gmail.com</t>
+  </si>
+  <si>
+    <t>85519994943</t>
+  </si>
+  <si>
+    <t>alexsantos_26032022110939@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -521,10 +527,10 @@
         <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>